<commit_message>
Revert to original OR files where customized to state
</commit_message>
<xml_diff>
--- a/InputData/elec/RM/Reserve Margin.xlsx
+++ b/InputData/elec/RM/Reserve Margin.xlsx
@@ -1,26 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI - units progress\InputData\elec\RM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jonah\Documents\EPS Model\.eps-oregon-1.4.3.2 - WIP\InputData\elec\RM\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8315521-6898-44B7-B29E-B858EAD3DD30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="11580"/>
+    <workbookView xWindow="28680" yWindow="-6480" windowWidth="15990" windowHeight="24990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="RM" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>RM Reserve Margin</t>
   </si>
@@ -28,21 +37,45 @@
     <t>Source:</t>
   </si>
   <si>
-    <t xml:space="preserve">North American Electrict Reliability Coorporation </t>
-  </si>
-  <si>
-    <t>http://www.nerc.com/pa/RAPA/ra/Reliability%20Assessments%20DL/2015_Summer_Reliability_Assessment.pdf</t>
-  </si>
-  <si>
-    <t>p.3, Table 1: Projected Demand, Resources, and Planning Reserve Margins, NERC Reference Margin Level (%)</t>
-  </si>
-  <si>
-    <t>2015 Summer Reliability Assessment</t>
-  </si>
-  <si>
     <t>Reserve Margin</t>
   </si>
   <si>
+    <t>Energy + Environmental Economics</t>
+  </si>
+  <si>
+    <t>Resource Adequacy in the Pacific Northwest</t>
+  </si>
+  <si>
+    <t>https://www.ethree.com/wp-content/uploads/2019/03/E3_Resource_Adequacy_in_the_Pacific-Northwest_March_2019.pdf</t>
+  </si>
+  <si>
+    <t>Page 36, Table 13. 2018 Reliability Statistics</t>
+  </si>
+  <si>
+    <t>PRM Requirement</t>
+  </si>
+  <si>
+    <t>Using E3's reports on the PNW as applicable to Oregon. The 12% PRM is slightly lower than the</t>
+  </si>
+  <si>
+    <t>usual ~15% found in the US and CA models. This makes sense due to the large presence of</t>
+  </si>
+  <si>
+    <t>hydroelectric power in the PNW and Oregon.</t>
+  </si>
+  <si>
+    <t>NERC backs up this lower PRM in its Reference Reserve Margin metric:</t>
+  </si>
+  <si>
+    <t>"If not provided, NERC assigned 15 percent Reserve Margin for predominately thermal systems and 10 percent for predominately hydro systems."</t>
+  </si>
+  <si>
+    <t>https://www.nerc.com/pa/RAPA/ri/Pages/PlanningReserveMargin.aspx</t>
+  </si>
+  <si>
+    <t>Following notes are copied from US EPS:</t>
+  </si>
+  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -53,16 +86,13 @@
   </si>
   <si>
     <t>changes in future reserve margin by year.</t>
-  </si>
-  <si>
-    <t>(dimensionless)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,13 +108,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -96,19 +147,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -199,6 +255,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -234,6 +307,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -409,94 +499,146 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B4" s="2">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B5" s="2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="D8" s="6">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{312A888B-A036-4EF9-A174-CA32801F6239}"/>
+    <hyperlink ref="A16" r:id="rId2" xr:uid="{BEFFC751-03E0-4620-82A5-083DBD3DAECB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AK2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>2015</v>
       </c>
@@ -606,117 +748,153 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="L2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="M2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="N2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="O2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="P2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="R2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="S2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="T2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="U2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="V2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="W2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="X2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="Y2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="Z2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="AA2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="AB2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="AC2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="AD2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="AE2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="AF2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="AG2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="AH2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="AI2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="AJ2" s="3">
-        <v>0.14119999999999999</v>
-      </c>
-      <c r="AK2" s="3">
-        <v>0.14119999999999999</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="C2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="D2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="E2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="F2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="G2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="H2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="I2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="J2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="K2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="L2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="M2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="N2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="O2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="P2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="Q2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="R2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="S2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="T2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="U2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="V2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="W2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="X2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="Y2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="Z2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="AA2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="AB2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="AC2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="AD2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="AE2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="AF2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="AG2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="AH2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="AI2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="AJ2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
+      </c>
+      <c r="AK2" s="2">
+        <f>About!$D$8</f>
+        <v>0.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>